<commit_message>
fix OpenAPI-Documentation for Post-Requests add MatrixStopStop-Template
</commit_message>
<xml_diff>
--- a/datentool_backend/indicators/tests/testdata/Reisezeitmatrix_Haltestelle_zu_Haltestelle.xlsx
+++ b/datentool_backend/indicators/tests/testdata/Reisezeitmatrix_Haltestelle_zu_Haltestelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.198.10\Projekte aktuell\JMG\20065 Datentool Daseinsvorsorge\30 Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\bule_datentool\datentool_backend\indicators\tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D724C67-1D4D-46CC-8F10-A5E02449F481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD2A1D-14F4-4B79-8EAD-756739D04D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C780C06-3521-4159-9AAB-AD1FD9D2C160}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0C780C06-3521-4159-9AAB-AD1FD9D2C160}"/>
   </bookViews>
   <sheets>
     <sheet name="Reisezeit" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Von Haltestelle (Nr)</t>
   </si>
@@ -44,6 +42,15 @@
   </si>
   <si>
     <t>Reisezeit in Minuten</t>
+  </si>
+  <si>
+    <t>from_stop</t>
+  </si>
+  <si>
+    <t>to_stop</t>
+  </si>
+  <si>
+    <t>minutes</t>
   </si>
 </sst>
 </file>
@@ -423,38 +430,141 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2172AB9-BF87-4E4D-8C29-7B8E510A2B95}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="10.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>77</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Bitte eine Zahl größer gleich 0 eintragen." sqref="C1:C1048576" xr:uid="{BD29B0DA-7558-43BF-9582-88E72FD6690A}">
+  <dataValidations count="3">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Bitte eine Zahl größer gleich 0 eintragen." sqref="C2 C3:C1048576" xr:uid="{BD29B0DA-7558-43BF-9582-88E72FD6690A}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Bitte eine ganze Zahl ab 0 eintragen, die der Nummer der Haltestelle laut Haltestellenliste entspricht." sqref="A1:B1048576" xr:uid="{2DD41ABA-E362-4C97-9401-FC697011F041}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Bitte eine ganze Zahl ab 0 eintragen, die der Nummer der Haltestelle laut Haltestellenliste entspricht." sqref="A2 B2" xr:uid="{2DD41ABA-E362-4C97-9401-FC697011F041}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:B1048576" xr:uid="{D77B9A4B-C436-478F-B783-CA98A6D3699A}">
+      <formula1>0</formula1>
+      <formula2>9999999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>